<commit_message>
Publish Update Part 1: Typed PC + Tag PC
</commit_message>
<xml_diff>
--- a/Experiment-Data/Experiment-Graphs-and-Tags/Experiment Datatable.xlsx
+++ b/Experiment-Data/Experiment-Graphs-and-Tags/Experiment Datatable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATENORDNER\Desktop\Stuff\Info_Zeug\Bachelor\8.Semester\Thesis\Experiment Datatable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C6D158-D1BE-4670-8810-8117564C0FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5954D3E-5F45-417E-A6F7-2575C9F0C850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{556AD7D9-BC17-4476-A761-6A17BECECEC6}"/>
   </bookViews>
@@ -929,23 +929,14 @@
     <t>Average Ranking</t>
   </si>
   <si>
-    <t>3.55, 3.5</t>
+    <t>3.5, 3.81</t>
   </si>
   <si>
-    <t>2.82, 3.13</t>
-  </si>
-  <si>
-    <t>2.64, 2.38</t>
-  </si>
-  <si>
-    <t>2.83, 2</t>
-  </si>
-  <si>
-    <t>2, 2</t>
+    <t>4.05, 4.06</t>
   </si>
   <si>
     <r>
-      <t>1.64</t>
+      <t>2.27</t>
     </r>
     <r>
       <rPr>
@@ -955,7 +946,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t>, 2.44</t>
+    </r>
+  </si>
+  <si>
+    <t>3,18, 3</t>
+  </si>
+  <si>
+    <t>3.17, 2.25</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.33, </t>
     </r>
     <r>
       <rPr>
@@ -966,7 +968,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.88</t>
+      <t>2.13</t>
     </r>
   </si>
 </sst>
@@ -1011,7 +1013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1021,6 +1023,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -16727,8 +16731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E322D54A-8F0A-4336-9477-BAD35E31194C}">
   <dimension ref="A2:AS173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AR20" sqref="AR20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17395,22 +17399,22 @@
         <v>176</v>
       </c>
       <c r="F18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>177</v>
-      </c>
       <c r="H18" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="I18" t="s">
+        <v>180</v>
+      </c>
+      <c r="J18" t="s">
+        <v>181</v>
+      </c>
+      <c r="K18" t="s">
         <v>182</v>
-      </c>
-      <c r="I18" t="s">
-        <v>179</v>
-      </c>
-      <c r="J18" t="s">
-        <v>180</v>
-      </c>
-      <c r="K18" t="s">
-        <v>181</v>
       </c>
       <c r="P18" t="s">
         <v>165</v>
@@ -18463,29 +18467,23 @@
       <c r="C37" t="s">
         <v>176</v>
       </c>
-      <c r="F37">
-        <f>(1 + 1 + 3 + 3 + 4 + 5 + 2 + 2 + 3 + 2 + 5)/11</f>
-        <v>2.8181818181818183</v>
-      </c>
-      <c r="G37">
-        <f>(1 + 1 + 3 + 3 + 3 + 5 + 4 + 6 + 1 + 6 + 6)/11</f>
-        <v>3.5454545454545454</v>
-      </c>
-      <c r="H37" s="4">
-        <f>(1 + 1 + 1 + 3 + 1 + 1 + 3 + 2 + 2 + 1 + 2)/11</f>
-        <v>1.6363636363636365</v>
-      </c>
-      <c r="I37">
-        <f>(1 + 1 + 6 + 3 + 1 + 4 + 1 + 2 + 4 + 5 + 1)/11</f>
-        <v>2.6363636363636362</v>
-      </c>
-      <c r="J37">
-        <f>(5 + 1 + 2 + 5 + 2 + 2)/6</f>
-        <v>2.8333333333333335</v>
-      </c>
-      <c r="K37">
-        <f>(2 + 2 + 3 + 1 + 2 + 2)/6</f>
-        <v>2</v>
+      <c r="F37" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="G37" s="7">
+        <v>4.05</v>
+      </c>
+      <c r="H37" s="8">
+        <v>2.27</v>
+      </c>
+      <c r="I37" s="7">
+        <v>3.18</v>
+      </c>
+      <c r="J37" s="7">
+        <v>3.17</v>
+      </c>
+      <c r="K37" s="7">
+        <v>2.33</v>
       </c>
     </row>
     <row r="44" spans="2:31" x14ac:dyDescent="0.25">
@@ -19047,28 +19045,22 @@
         <v>176</v>
       </c>
       <c r="F57">
-        <f>(3 + 1 + 3 + 3 + 4 + 6 + 2 + 3)/8</f>
-        <v>3.125</v>
+        <v>3.81</v>
       </c>
       <c r="G57">
-        <f>(3 + 1 + 3 + 3 + 3 + 5 + 4 + 6)/8</f>
-        <v>3.5</v>
-      </c>
-      <c r="H57" s="4">
-        <f>(1 + 1 + 1 + 3 + 2 + 1 + 3 + 3)/8</f>
-        <v>1.875</v>
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="H57">
+        <v>2.44</v>
       </c>
       <c r="I57">
-        <f>(1 + 1 + 6 + 3 + 1 + 3 + 1 + 3)/8</f>
-        <v>2.375</v>
+        <v>3</v>
       </c>
       <c r="J57">
-        <f>(3 + 1 + 2 + 2)/4</f>
-        <v>2</v>
-      </c>
-      <c r="K57">
-        <f>(2 + 2 + 3 + 1)/4</f>
-        <v>2</v>
+        <v>2.25</v>
+      </c>
+      <c r="K57" s="4">
+        <v>2.13</v>
       </c>
     </row>
     <row r="59" spans="2:22" x14ac:dyDescent="0.25">

</xml_diff>